<commit_message>
Update business scraper plan.xlsx
</commit_message>
<xml_diff>
--- a/documents/business scraper plan.xlsx
+++ b/documents/business scraper plan.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gingg\Documents\GitHub\bolar\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7606E7B1-F793-4550-B8DE-FD7DE8C47134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CABE287-F479-4294-8CE9-E47B8C5150E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F65CDB09-F7AD-4761-AB37-8B010387F582}"/>
+    <workbookView xWindow="345" yWindow="1575" windowWidth="19200" windowHeight="12405" activeTab="2" xr2:uid="{F65CDB09-F7AD-4761-AB37-8B010387F582}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="110">
   <si>
     <t>Shared Plus Hosting</t>
   </si>
@@ -320,6 +322,54 @@
   </si>
   <si>
     <t>domein</t>
+  </si>
+  <si>
+    <t>Worklog</t>
+  </si>
+  <si>
+    <t>Sended 83 emails</t>
+  </si>
+  <si>
+    <t>at 13:52</t>
+  </si>
+  <si>
+    <t>1min</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>Took</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Find template</t>
+  </si>
+  <si>
+    <t>Build Django Site and host</t>
+  </si>
+  <si>
+    <t>Hubspot email campaine komt in spam terecht, build email bot dat niet in spam komt</t>
+  </si>
+  <si>
+    <t>12h</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>Sendded mail</t>
+  </si>
+  <si>
+    <t>Check 1 week later Conversie</t>
   </si>
 </sst>
 </file>
@@ -327,11 +377,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="_-[$€-2]\ * #,##0_-;\-[$€-2]\ * #,##0_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="_-[$€-2]\ * #,##0_-;\-[$€-2]\ * #,##0_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -412,28 +462,29 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -769,11 +820,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A449F407-5671-4298-9D79-D2407E4A29DF}">
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
+        <v>45374</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>45397</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>45398</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>45399</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H20" s="18">
+        <v>45396</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H21" s="18">
+        <v>45397</v>
+      </c>
+      <c r="I21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H22" s="18">
+        <v>45398</v>
+      </c>
+      <c r="I22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H23" s="18">
+        <v>45399</v>
+      </c>
+      <c r="J23" t="s">
+        <v>108</v>
+      </c>
+      <c r="M23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D7762B-738E-4C31-B036-23C8D83BCAF8}">
   <dimension ref="B2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,10 +1065,10 @@
       </c>
       <c r="C12">
         <f>ROUND(C10*D12,0)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D12" s="7">
-        <v>3.2000000000000001E-2</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -911,7 +1086,7 @@
       </c>
       <c r="C15" s="9">
         <f>C14*C12</f>
-        <v>1781.25</v>
+        <v>5937.5</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
@@ -920,7 +1095,7 @@
       </c>
       <c r="C16" s="1">
         <f>C15*21%</f>
-        <v>374.0625</v>
+        <v>1246.875</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -929,7 +1104,7 @@
       </c>
       <c r="C17" s="2">
         <f>C15/ (AVERAGE(Sheet3!D14:F14))</f>
-        <v>1775.3322259136212</v>
+        <v>5917.7740863787367</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -938,7 +1113,7 @@
       </c>
       <c r="C18" s="1">
         <f>C17/10000 * 49</f>
-        <v>8.6991279069767433</v>
+        <v>28.997093023255808</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -962,11 +1137,11 @@
       </c>
       <c r="C21" s="1">
         <f>C15-C16-C18-C19</f>
-        <v>1344.4883720930231</v>
+        <v>4607.6279069767443</v>
       </c>
       <c r="D21" s="10">
         <f>C21/C15</f>
-        <v>0.75480048959608315</v>
+        <v>0.77602154222766218</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -1027,7 +1202,7 @@
       </c>
       <c r="C37" s="1">
         <f>C21+C36</f>
-        <v>394.48837209302314</v>
+        <v>3657.6279069767443</v>
       </c>
     </row>
   </sheetData>
@@ -1035,12 +1210,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D050417B-3273-4955-A7A8-F9E9DF39BEC5}">
   <dimension ref="A1:Y59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,99 +1311,99 @@
       </c>
       <c r="B2" s="17">
         <f>B22</f>
-        <v>221.34534883720931</v>
+        <v>213.22616279069769</v>
       </c>
       <c r="C2" s="17">
-        <f>C22+B2</f>
-        <v>1212.7707122093022</v>
+        <f t="shared" ref="C2:Y2" si="0">C22+B2</f>
+        <v>1167.1002906976746</v>
       </c>
       <c r="D2" s="17">
-        <f>D22+C2</f>
-        <v>3368.0558466569764</v>
+        <f t="shared" si="0"/>
+        <v>3242.1577180232562</v>
       </c>
       <c r="E2" s="17">
-        <f>E22+D2</f>
-        <v>6994.2193125726735</v>
+        <f t="shared" si="0"/>
+        <v>6708.3133398255814</v>
       </c>
       <c r="F2" s="17">
-        <f>F22+E2</f>
-        <v>12728.256636308139</v>
+        <f t="shared" si="0"/>
+        <v>12218.468776860464</v>
       </c>
       <c r="G2" s="17">
-        <f>G22+F2</f>
-        <v>20463.063696247093</v>
+        <f t="shared" si="0"/>
+        <v>19666.711966406976</v>
       </c>
       <c r="H2" s="17">
-        <f>H22+G2</f>
-        <v>33517.732309314539</v>
+        <f t="shared" si="0"/>
+        <v>32248.553901765117</v>
       </c>
       <c r="I2" s="17">
-        <f>I22+H2</f>
-        <v>44197.849173987794</v>
+        <f t="shared" si="0"/>
+        <v>42399.966729909305</v>
       </c>
       <c r="J2" s="17">
-        <f>J22+I2</f>
-        <v>58552.226210975583</v>
+        <f t="shared" si="0"/>
+        <v>56173.343492818611</v>
       </c>
       <c r="K2" s="17">
-        <f>K22+J2</f>
-        <v>75660.002229469479</v>
+        <f t="shared" si="0"/>
+        <v>72641.494374273258</v>
       </c>
       <c r="L2" s="17">
-        <f>L22+K2</f>
-        <v>95709.745180576894</v>
+        <f t="shared" si="0"/>
+        <v>91965.465454535472</v>
       </c>
       <c r="M2" s="17">
-        <f>M22+L2</f>
-        <v>110842.82014450269</v>
+        <f t="shared" si="0"/>
+        <v>106305.33762257356</v>
       </c>
       <c r="N2" s="17">
-        <f>N22+M2</f>
-        <v>132696.58175437257</v>
+        <f t="shared" si="0"/>
+        <v>127259.10829961585</v>
       </c>
       <c r="O2" s="17">
-        <f>O22+N2</f>
-        <v>158962.33058256333</v>
+        <f t="shared" si="0"/>
+        <v>152538.99538232305</v>
       </c>
       <c r="P2" s="17">
-        <f>P22+O2</f>
-        <v>188999.34046177499</v>
+        <f t="shared" si="0"/>
+        <v>181490.37380739755</v>
       </c>
       <c r="Q2" s="17">
-        <f>Q22+P2</f>
-        <v>212273.75935486919</v>
+        <f t="shared" si="0"/>
+        <v>203548.08453156272</v>
       </c>
       <c r="R2" s="17">
-        <f>R22+Q2</f>
-        <v>244795.13769676513</v>
+        <f t="shared" si="0"/>
+        <v>234730.3820448081</v>
       </c>
       <c r="S2" s="17">
-        <f>S22+R2</f>
-        <v>283795.09605375963</v>
+        <f t="shared" si="0"/>
+        <v>272265.11975491914</v>
       </c>
       <c r="T2" s="17">
-        <f>T22+S2</f>
-        <v>329244.87930202432</v>
+        <f t="shared" si="0"/>
+        <v>316072.94384253281</v>
       </c>
       <c r="U2" s="17">
-        <f>U22+T2</f>
-        <v>363618.50028662174</v>
+        <f t="shared" si="0"/>
+        <v>348651.28292122338</v>
       </c>
       <c r="V2" s="17">
-        <f>V22+U2</f>
-        <v>410645.81543008325</v>
+        <f t="shared" si="0"/>
+        <v>393741.70129777794</v>
       </c>
       <c r="W2" s="17">
-        <f>W22+V2</f>
-        <v>465029.05904832564</v>
+        <f t="shared" si="0"/>
+        <v>446084.7639744273</v>
       </c>
       <c r="X2" s="17">
-        <f>X22+W2</f>
-        <v>524029.09829930728</v>
+        <f t="shared" si="0"/>
+        <v>502960.50345228688</v>
       </c>
       <c r="Y2" s="17">
-        <f>Y22+X2</f>
-        <v>565479.19815735624</v>
+        <f t="shared" si="0"/>
+        <v>542179.29063307715</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1327,95 +1502,95 @@
       </c>
       <c r="C6" s="9">
         <f>B25</f>
-        <v>774.70872093023263</v>
+        <v>746.29156976744184</v>
       </c>
       <c r="D6" s="9">
-        <f t="shared" ref="D6:Y6" si="0">C25</f>
-        <v>2577.7059447674419</v>
+        <f t="shared" ref="D6:Y6" si="1">C25</f>
+        <v>2480.0727325581397</v>
       </c>
       <c r="E6" s="9">
-        <f t="shared" si="0"/>
-        <v>5603.741349563953</v>
+        <f t="shared" si="1"/>
+        <v>5395.1493110465117</v>
       </c>
       <c r="F6" s="9">
         <f>E25</f>
-        <v>7252.326931831396</v>
+        <v>6932.3112436046504</v>
       </c>
       <c r="G6" s="9">
-        <f t="shared" si="0"/>
-        <v>11468.074647470932</v>
+        <f t="shared" si="1"/>
+        <v>11020.310874069766</v>
       </c>
       <c r="H6" s="9">
-        <f t="shared" si="0"/>
-        <v>15469.614119877908</v>
+        <f t="shared" si="1"/>
+        <v>14896.486379093025</v>
       </c>
       <c r="I6" s="9">
-        <f t="shared" si="0"/>
-        <v>16318.335766334303</v>
+        <f t="shared" si="1"/>
+        <v>15727.302419197673</v>
       </c>
       <c r="J6" s="9">
-        <f t="shared" si="0"/>
-        <v>13350.146080841569</v>
+        <f t="shared" si="1"/>
+        <v>12689.26603518023</v>
       </c>
       <c r="K6" s="9">
-        <f t="shared" si="0"/>
-        <v>17942.97129623474</v>
+        <f t="shared" si="1"/>
+        <v>17216.720953636624</v>
       </c>
       <c r="L6" s="9">
-        <f t="shared" si="0"/>
-        <v>21384.72002311737</v>
+        <f t="shared" si="1"/>
+        <v>20585.188601818314</v>
       </c>
       <c r="M6" s="9">
-        <f t="shared" si="0"/>
-        <v>25062.178688884269</v>
+        <f t="shared" si="1"/>
+        <v>24154.963850327757</v>
       </c>
       <c r="N6" s="9">
-        <f t="shared" si="0"/>
-        <v>18916.343704907249</v>
+        <f t="shared" si="1"/>
+        <v>17924.840210047598</v>
       </c>
       <c r="O6" s="9">
-        <f t="shared" si="0"/>
-        <v>27317.20201233734</v>
+        <f t="shared" si="1"/>
+        <v>26192.213346302862</v>
       </c>
       <c r="P6" s="9">
-        <f t="shared" si="0"/>
-        <v>32832.186035238432</v>
+        <f t="shared" si="1"/>
+        <v>31599.858853383979</v>
       </c>
       <c r="Q6" s="9">
-        <f t="shared" si="0"/>
-        <v>37546.262349014563</v>
+        <f t="shared" si="1"/>
+        <v>36189.22303134315</v>
       </c>
       <c r="R6" s="9">
-        <f t="shared" si="0"/>
-        <v>29093.02361636774</v>
+        <f t="shared" si="1"/>
+        <v>27572.13840520646</v>
       </c>
       <c r="S6" s="9">
-        <f t="shared" si="0"/>
-        <v>40651.722927369919</v>
+        <f t="shared" si="1"/>
+        <v>38977.871891556715</v>
       </c>
       <c r="T6" s="9">
-        <f t="shared" si="0"/>
-        <v>48749.947946243097</v>
+        <f t="shared" si="1"/>
+        <v>46918.422137638816</v>
       </c>
       <c r="U6" s="9">
-        <f t="shared" si="0"/>
-        <v>56812.229060330836</v>
+        <f t="shared" si="1"/>
+        <v>54759.780109517073</v>
       </c>
       <c r="V6" s="9">
-        <f t="shared" si="0"/>
-        <v>42967.026230746815</v>
+        <f t="shared" si="1"/>
+        <v>40722.923848363178</v>
       </c>
       <c r="W6" s="9">
-        <f t="shared" si="0"/>
-        <v>58784.143929326892</v>
+        <f t="shared" si="1"/>
+        <v>56363.022970693215</v>
       </c>
       <c r="X6" s="9">
-        <f t="shared" si="0"/>
-        <v>67979.054522802981</v>
+        <f t="shared" si="1"/>
+        <v>65428.828345811722</v>
       </c>
       <c r="Y6" s="9">
-        <f t="shared" si="0"/>
-        <v>73750.04906372707</v>
+        <f t="shared" si="1"/>
+        <v>71094.674347324471</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -1587,96 +1762,96 @@
         <v>50</v>
       </c>
       <c r="C9" s="15">
-        <f t="shared" ref="C9:Y9" si="1">C6-C7-C8</f>
-        <v>574.70872093023263</v>
+        <f t="shared" ref="C9:Y9" si="2">C6-C7-C8</f>
+        <v>546.29156976744184</v>
       </c>
       <c r="D9" s="15">
-        <f t="shared" si="1"/>
-        <v>2227.7059447674419</v>
+        <f t="shared" si="2"/>
+        <v>2130.0727325581397</v>
       </c>
       <c r="E9" s="15">
-        <f t="shared" si="1"/>
-        <v>2634.928849563953</v>
+        <f t="shared" si="2"/>
+        <v>2426.3368110465117</v>
       </c>
       <c r="F9" s="15">
-        <f t="shared" si="1"/>
-        <v>6602.326931831396</v>
+        <f t="shared" si="2"/>
+        <v>6282.3112436046504</v>
       </c>
       <c r="G9" s="15">
-        <f t="shared" si="1"/>
-        <v>10768.074647470932</v>
+        <f t="shared" si="2"/>
+        <v>10320.310874069766</v>
       </c>
       <c r="H9" s="15">
-        <f t="shared" si="1"/>
-        <v>14619.614119877908</v>
+        <f t="shared" si="2"/>
+        <v>14046.486379093025</v>
       </c>
       <c r="I9" s="15">
-        <f t="shared" si="1"/>
-        <v>5069.0232663343031</v>
+        <f t="shared" si="2"/>
+        <v>4477.9899191976729</v>
       </c>
       <c r="J9" s="15">
-        <f t="shared" si="1"/>
-        <v>12250.146080841569</v>
+        <f t="shared" si="2"/>
+        <v>11589.26603518023</v>
       </c>
       <c r="K9" s="15">
-        <f t="shared" si="1"/>
-        <v>16742.97129623474</v>
+        <f t="shared" si="2"/>
+        <v>16016.720953636624</v>
       </c>
       <c r="L9" s="15">
-        <f t="shared" si="1"/>
-        <v>19984.72002311737</v>
+        <f t="shared" si="2"/>
+        <v>19185.188601818314</v>
       </c>
       <c r="M9" s="15">
-        <f t="shared" si="1"/>
-        <v>5632.1161888842689</v>
+        <f t="shared" si="2"/>
+        <v>4724.9013503277565</v>
       </c>
       <c r="N9" s="15">
-        <f t="shared" si="1"/>
-        <v>17266.343704907249</v>
+        <f t="shared" si="2"/>
+        <v>16274.840210047598</v>
       </c>
       <c r="O9" s="15">
-        <f t="shared" si="1"/>
-        <v>25567.20201233734</v>
+        <f t="shared" si="2"/>
+        <v>24442.213346302862</v>
       </c>
       <c r="P9" s="15">
-        <f t="shared" si="1"/>
-        <v>30882.186035238432</v>
+        <f t="shared" si="2"/>
+        <v>29649.858853383979</v>
       </c>
       <c r="Q9" s="15">
-        <f t="shared" si="1"/>
-        <v>8027.2310990145634</v>
+        <f t="shared" si="2"/>
+        <v>6670.1917813431501</v>
       </c>
       <c r="R9" s="15">
-        <f t="shared" si="1"/>
-        <v>26693.02361636774</v>
+        <f t="shared" si="2"/>
+        <v>25172.13840520646</v>
       </c>
       <c r="S9" s="15">
-        <f t="shared" si="1"/>
-        <v>38051.722927369919</v>
+        <f t="shared" si="2"/>
+        <v>36377.871891556715</v>
       </c>
       <c r="T9" s="15">
-        <f t="shared" si="1"/>
-        <v>45949.947946243097</v>
+        <f t="shared" si="2"/>
+        <v>44118.422137638816</v>
       </c>
       <c r="U9" s="15">
-        <f t="shared" si="1"/>
-        <v>13026.947810330836</v>
+        <f t="shared" si="2"/>
+        <v>10974.498859517073</v>
       </c>
       <c r="V9" s="15">
-        <f t="shared" si="1"/>
-        <v>39767.026230746815</v>
+        <f t="shared" si="2"/>
+        <v>37522.923848363178</v>
       </c>
       <c r="W9" s="15">
-        <f t="shared" si="1"/>
-        <v>55484.143929326892</v>
+        <f t="shared" si="2"/>
+        <v>53063.022970693215</v>
       </c>
       <c r="X9" s="15">
-        <f t="shared" si="1"/>
-        <v>64579.054522802981</v>
+        <f t="shared" si="2"/>
+        <v>62028.828345811722</v>
       </c>
       <c r="Y9" s="15">
-        <f t="shared" si="1"/>
-        <v>16035.67406372707</v>
+        <f t="shared" si="2"/>
+        <v>13380.299347324471</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -1722,87 +1897,87 @@
         <v>6887.5</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" ref="E11:Y11" si="2">E41+E47</f>
+        <f t="shared" ref="E11:Y11" si="3">E41+E47</f>
         <v>10153.125</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13418.75</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16090.625</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19296.875</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23156.25</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25293.75</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27846.875</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32240.625</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34437.5</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39959.375</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42868.75</v>
       </c>
       <c r="P11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47262.5</v>
       </c>
       <c r="Q11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>53615.625</v>
       </c>
       <c r="R11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>58365.625</v>
       </c>
       <c r="S11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>63531.25</v>
       </c>
       <c r="T11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>72318.75</v>
       </c>
       <c r="U11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77900</v>
       </c>
       <c r="V11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83125</v>
       </c>
       <c r="W11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85975</v>
       </c>
       <c r="X11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88587.5</v>
       </c>
       <c r="Y11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>93575</v>
       </c>
     </row>
@@ -1913,99 +2088,99 @@
       </c>
       <c r="B13" s="1">
         <f>Sheet1!$C$18 * B39</f>
-        <v>17.398255813953487</v>
+        <v>57.994186046511615</v>
       </c>
       <c r="C13" s="1">
         <f>Sheet1!$C$18 * C39</f>
-        <v>52.194767441860463</v>
+        <v>173.98255813953483</v>
       </c>
       <c r="D13" s="1">
         <f>Sheet1!$C$18 * D39</f>
-        <v>95.690406976744171</v>
+        <v>318.96802325581388</v>
       </c>
       <c r="E13" s="1">
         <f>Sheet1!$C$18 * E39</f>
-        <v>139.18604651162789</v>
+        <v>463.95348837209292</v>
       </c>
       <c r="F13" s="1">
         <f>Sheet1!$C$18 * F39</f>
-        <v>182.6816860465116</v>
+        <v>608.93895348837191</v>
       </c>
       <c r="G13" s="1">
         <f>Sheet1!$C$18 * G39</f>
-        <v>217.4781976744186</v>
+        <v>724.92732558139517</v>
       </c>
       <c r="H13" s="1">
         <f>Sheet1!$C$18 * H39</f>
-        <v>260.9738372093023</v>
+        <v>869.91279069767427</v>
       </c>
       <c r="I13" s="1">
         <f>Sheet1!$C$18 * I39</f>
-        <v>313.16860465116275</v>
+        <v>1043.895348837209</v>
       </c>
       <c r="J13" s="1">
         <f>Sheet1!$C$18 * J39</f>
-        <v>339.26598837209298</v>
+        <v>1130.8866279069764</v>
       </c>
       <c r="K13" s="1">
         <f>Sheet1!$C$18 * K39</f>
-        <v>374.06249999999994</v>
+        <v>1246.8749999999998</v>
       </c>
       <c r="L13" s="1">
         <f>Sheet1!$C$18 * L39</f>
-        <v>434.95639534883719</v>
+        <v>1449.8546511627903</v>
       </c>
       <c r="M13" s="1">
         <f>Sheet1!$C$18 * M39</f>
-        <v>461.05377906976742</v>
+        <v>1536.8459302325577</v>
       </c>
       <c r="N13" s="1">
         <f>Sheet1!$C$18 * N39</f>
-        <v>539.34593023255809</v>
+        <v>1797.81976744186</v>
       </c>
       <c r="O13" s="1">
         <f>Sheet1!$C$18 * O39</f>
-        <v>574.14244186046506</v>
+        <v>1913.8081395348834</v>
       </c>
       <c r="P13" s="1">
         <f>Sheet1!$C$18 * P39</f>
-        <v>635.03633720930225</v>
+        <v>2116.7877906976742</v>
       </c>
       <c r="Q13" s="1">
         <f>Sheet1!$C$18 * Q39</f>
-        <v>722.02761627906966</v>
+        <v>2406.7587209302319</v>
       </c>
       <c r="R13" s="1">
         <f>Sheet1!$C$18 * R39</f>
-        <v>782.92151162790685</v>
+        <v>2609.7383720930225</v>
       </c>
       <c r="S13" s="1">
         <f>Sheet1!$C$18 * S39</f>
-        <v>852.5145348837209</v>
+        <v>2841.7151162790692</v>
       </c>
       <c r="T13" s="1">
         <f>Sheet1!$C$18 * T39</f>
-        <v>974.30232558139528</v>
+        <v>3247.6744186046503</v>
       </c>
       <c r="U13" s="1">
         <f>Sheet1!$C$18 * U39</f>
-        <v>1043.8953488372092</v>
+        <v>3479.6511627906971</v>
       </c>
       <c r="V13" s="1">
         <f>Sheet1!$C$18 * V39</f>
-        <v>1113.4883720930231</v>
+        <v>3711.6279069767434</v>
       </c>
       <c r="W13" s="1">
         <f>Sheet1!$C$18 * W39</f>
-        <v>1148.2848837209301</v>
+        <v>3827.6162790697667</v>
       </c>
       <c r="X13" s="1">
         <f>Sheet1!$C$18 * X39</f>
-        <v>1183.0813953488371</v>
+        <v>3943.6046511627897</v>
       </c>
       <c r="Y13" s="1">
         <f>Sheet1!$C$18 * Y39</f>
-        <v>1252.674418604651</v>
+        <v>4175.5813953488359</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -2013,99 +2188,99 @@
         <v>77</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" ref="B14:Y14" si="3">B11*5%</f>
+        <f t="shared" ref="B14:Y14" si="4">B11*5%</f>
         <v>59.375</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>184.0625</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>344.375</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>507.65625</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>670.9375</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>804.53125</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>964.84375</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1157.8125</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1264.6875</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1392.34375</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1612.03125</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1721.875</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1997.96875</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2143.4375</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2363.125</v>
       </c>
       <c r="Q14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2680.78125</v>
       </c>
       <c r="R14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2918.28125</v>
       </c>
       <c r="S14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3176.5625</v>
       </c>
       <c r="T14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3615.9375</v>
       </c>
       <c r="U14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3895</v>
       </c>
       <c r="V14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4156.25</v>
       </c>
       <c r="W14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4298.75</v>
       </c>
       <c r="X14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4429.375</v>
       </c>
       <c r="Y14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4678.75</v>
       </c>
     </row>
@@ -2141,99 +2316,99 @@
       </c>
       <c r="B16" s="9">
         <f>B11-B13-B12-B14</f>
-        <v>1056.7267441860465</v>
+        <v>1016.1308139534883</v>
       </c>
       <c r="C16" s="9">
-        <f t="shared" ref="C16:D16" si="4">C11-C13-C12-C14</f>
-        <v>3390.9927325581393</v>
+        <f>C11-C13-C12-C14</f>
+        <v>3269.2049418604652</v>
       </c>
       <c r="D16" s="9">
-        <f t="shared" si="4"/>
-        <v>6393.4345930232557</v>
+        <f>D11-D13-D12-D14</f>
+        <v>6170.1569767441861</v>
       </c>
       <c r="E16" s="9">
         <f>E11-E13-E12-E14</f>
-        <v>9452.2827034883721</v>
+        <v>9127.5152616279065</v>
       </c>
       <c r="F16" s="9">
         <f t="shared" ref="F16:Y16" si="5">F11-F13-F12-F14</f>
-        <v>12511.130813953489</v>
+        <v>12084.873546511628</v>
       </c>
       <c r="G16" s="9">
         <f t="shared" si="5"/>
-        <v>15014.615552325582</v>
+        <v>14507.166424418605</v>
       </c>
       <c r="H16" s="9">
         <f t="shared" si="5"/>
-        <v>18017.057412790698</v>
+        <v>17408.118459302324</v>
       </c>
       <c r="I16" s="9">
         <f t="shared" si="5"/>
-        <v>21631.268895348836</v>
+        <v>20900.54215116279</v>
       </c>
       <c r="J16" s="9">
         <f t="shared" si="5"/>
-        <v>23635.796511627908</v>
+        <v>22844.175872093023</v>
       </c>
       <c r="K16" s="9">
         <f t="shared" si="5"/>
-        <v>26026.46875</v>
+        <v>25153.65625</v>
       </c>
       <c r="L16" s="9">
         <f t="shared" si="5"/>
-        <v>30139.637354651164</v>
+        <v>29124.73909883721</v>
       </c>
       <c r="M16" s="9">
         <f t="shared" si="5"/>
-        <v>32200.571220930229</v>
+        <v>31124.779069767443</v>
       </c>
       <c r="N16" s="9">
         <f t="shared" si="5"/>
-        <v>37368.060319767443</v>
+        <v>36109.586482558138</v>
       </c>
       <c r="O16" s="9">
         <f t="shared" si="5"/>
-        <v>40097.170058139534</v>
+        <v>38757.504360465115</v>
       </c>
       <c r="P16" s="9">
         <f t="shared" si="5"/>
-        <v>44210.338662790695</v>
+        <v>42728.587209302328</v>
       </c>
       <c r="Q16" s="9">
         <f t="shared" si="5"/>
-        <v>50158.816133720931</v>
+        <v>48474.085029069771</v>
       </c>
       <c r="R16" s="9">
         <f t="shared" si="5"/>
-        <v>54610.422238372092</v>
+        <v>52783.605377906977</v>
       </c>
       <c r="S16" s="9">
         <f t="shared" si="5"/>
-        <v>59448.172965116282</v>
+        <v>57458.972383720931</v>
       </c>
       <c r="T16" s="9">
         <f t="shared" si="5"/>
-        <v>67674.51017441861</v>
+        <v>65401.138081395344</v>
       </c>
       <c r="U16" s="9">
         <f t="shared" si="5"/>
-        <v>72907.104651162794</v>
+        <v>70471.348837209298</v>
       </c>
       <c r="V16" s="9">
         <f t="shared" si="5"/>
-        <v>77801.261627906977</v>
+        <v>75203.122093023252</v>
       </c>
       <c r="W16" s="9">
         <f t="shared" si="5"/>
-        <v>80473.965116279069</v>
+        <v>77794.633720930229</v>
       </c>
       <c r="X16" s="9">
         <f t="shared" si="5"/>
-        <v>82921.04360465116</v>
+        <v>80160.520348837206</v>
       </c>
       <c r="Y16" s="9">
         <f t="shared" si="5"/>
-        <v>87589.575581395344</v>
+        <v>84666.66860465116</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -2242,99 +2417,99 @@
       </c>
       <c r="B17" s="10">
         <f>(B16-B11*21%)/B11</f>
-        <v>0.67987515299877599</v>
+        <v>0.64568910648714806</v>
       </c>
       <c r="C17" s="10">
         <f t="shared" ref="C17:Y17" si="6">(C16-C11*21%)/C11</f>
-        <v>0.71115252497334858</v>
+        <v>0.67806925415564423</v>
       </c>
       <c r="D17" s="10">
         <f t="shared" si="6"/>
-        <v>0.71826636559321322</v>
+        <v>0.68584856286666951</v>
       </c>
       <c r="E17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72097275011273598</v>
+        <v>0.68898580600828874</v>
       </c>
       <c r="F17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72236186783072109</v>
+        <v>0.69059607239956244</v>
       </c>
       <c r="G17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72312817571260168</v>
+        <v>0.69159123243619214</v>
       </c>
       <c r="H17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72367746916486209</v>
+        <v>0.69212111853874392</v>
       </c>
       <c r="I17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72414386592599567</v>
+        <v>0.69258751529987761</v>
       </c>
       <c r="J17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72445204889065118</v>
+        <v>0.69315496405606214</v>
       </c>
       <c r="K17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72462798788014815</v>
+        <v>0.69328470429805855</v>
       </c>
       <c r="L17" s="10">
         <f t="shared" si="6"/>
-        <v>0.7248341527079939</v>
+        <v>0.69335528851680794</v>
       </c>
       <c r="M17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72504381040813737</v>
+        <v>0.69380483687164984</v>
       </c>
       <c r="N17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72515127100379928</v>
+        <v>0.69365743915059075</v>
       </c>
       <c r="O17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72534731145973541</v>
+        <v>0.69409690883137753</v>
       </c>
       <c r="P17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72542107723439719</v>
+        <v>0.69406955216720079</v>
       </c>
       <c r="Q17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72552609213677788</v>
+        <v>0.69410370165543667</v>
       </c>
       <c r="R17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72566071190657333</v>
+        <v>0.69436117796917241</v>
       </c>
       <c r="S17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72573120259897739</v>
+        <v>0.69442061794346766</v>
       </c>
       <c r="T17" s="10">
         <f t="shared" si="6"/>
-        <v>0.7257809720773466</v>
+        <v>0.69434552700918284</v>
       </c>
       <c r="U17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72590634982237223</v>
+        <v>0.6946386243544197</v>
       </c>
       <c r="V17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72595502710264037</v>
+        <v>0.69469921314915195</v>
       </c>
       <c r="W17" s="10">
         <f t="shared" si="6"/>
-        <v>0.7260158780608208</v>
+        <v>0.69485180251154677</v>
       </c>
       <c r="X17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72603548587160893</v>
+        <v>0.69487394213446829</v>
       </c>
       <c r="Y17" s="10">
         <f t="shared" si="6"/>
-        <v>0.72603607353882282</v>
+        <v>0.69480009195459425</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -2369,100 +2544,100 @@
         <v>80</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" ref="B21:C21" si="7">B9+B16</f>
-        <v>1106.7267441860465</v>
+        <f>B9+B16</f>
+        <v>1066.1308139534883</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="7"/>
-        <v>3965.701453488372</v>
+        <f>C9+C16</f>
+        <v>3815.4965116279072</v>
       </c>
       <c r="D21" s="1">
         <f>D9+D16</f>
-        <v>8621.1405377906976</v>
+        <v>8300.2297093023262</v>
       </c>
       <c r="E21" s="1">
         <f>E9+E16</f>
-        <v>12087.211553052326</v>
+        <v>11553.852072674417</v>
       </c>
       <c r="F21" s="1">
         <f>F9+F16</f>
-        <v>19113.457745784886</v>
+        <v>18367.184790116276</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" ref="G21:Y21" si="8">G9+G16</f>
-        <v>25782.690199796514</v>
+        <f t="shared" ref="G21:Y21" si="7">G9+G16</f>
+        <v>24827.477298488371</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="8"/>
-        <v>32636.671532668606</v>
+        <f t="shared" si="7"/>
+        <v>31454.604838395349</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="8"/>
-        <v>26700.292161683137</v>
+        <f t="shared" si="7"/>
+        <v>25378.532070360463</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="8"/>
-        <v>35885.942592469481</v>
+        <f t="shared" si="7"/>
+        <v>34433.441907273256</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="8"/>
-        <v>42769.44004623474</v>
+        <f t="shared" si="7"/>
+        <v>41170.377203636628</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="8"/>
-        <v>50124.357377768538</v>
+        <f t="shared" si="7"/>
+        <v>48309.92770065552</v>
       </c>
       <c r="M21" s="1">
-        <f t="shared" si="8"/>
-        <v>37832.687409814498</v>
+        <f t="shared" si="7"/>
+        <v>35849.680420095203</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="8"/>
-        <v>54634.404024674688</v>
+        <f t="shared" si="7"/>
+        <v>52384.426692605732</v>
       </c>
       <c r="O21" s="1">
-        <f t="shared" si="8"/>
-        <v>65664.372070476878</v>
+        <f t="shared" si="7"/>
+        <v>63199.717706767973</v>
       </c>
       <c r="P21" s="1">
-        <f t="shared" si="8"/>
-        <v>75092.524698029127</v>
+        <f t="shared" si="7"/>
+        <v>72378.4460626863</v>
       </c>
       <c r="Q21" s="1">
-        <f t="shared" si="8"/>
-        <v>58186.047232735495</v>
+        <f t="shared" si="7"/>
+        <v>55144.276810412921</v>
       </c>
       <c r="R21" s="1">
-        <f t="shared" si="8"/>
-        <v>81303.445854739839</v>
+        <f t="shared" si="7"/>
+        <v>77955.74378311343</v>
       </c>
       <c r="S21" s="1">
-        <f t="shared" si="8"/>
-        <v>97499.895892486209</v>
+        <f t="shared" si="7"/>
+        <v>93836.844275277646</v>
       </c>
       <c r="T21" s="1">
-        <f t="shared" si="8"/>
-        <v>113624.4581206617</v>
+        <f t="shared" si="7"/>
+        <v>109519.56021903416</v>
       </c>
       <c r="U21" s="1">
-        <f t="shared" si="8"/>
-        <v>85934.052461493629</v>
+        <f t="shared" si="7"/>
+        <v>81445.84769672637</v>
       </c>
       <c r="V21" s="1">
-        <f t="shared" si="8"/>
-        <v>117568.28785865378</v>
+        <f t="shared" si="7"/>
+        <v>112726.04594138643</v>
       </c>
       <c r="W21" s="1">
-        <f t="shared" si="8"/>
-        <v>135958.10904560596</v>
+        <f t="shared" si="7"/>
+        <v>130857.65669162344</v>
       </c>
       <c r="X21" s="1">
-        <f t="shared" si="8"/>
-        <v>147500.09812745414</v>
+        <f t="shared" si="7"/>
+        <v>142189.34869464894</v>
       </c>
       <c r="Y21" s="1">
-        <f t="shared" si="8"/>
-        <v>103625.24964512241</v>
+        <f t="shared" si="7"/>
+        <v>98046.967951975632</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -2471,99 +2646,99 @@
       </c>
       <c r="B22" s="1">
         <f>B21*B23</f>
-        <v>221.34534883720931</v>
+        <v>213.22616279069769</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" ref="C22:Y22" si="9">C21*C23</f>
-        <v>991.42536337209299</v>
+        <f t="shared" ref="C22:Y22" si="8">C21*C23</f>
+        <v>953.87412790697681</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="9"/>
-        <v>2155.2851344476744</v>
+        <f t="shared" si="8"/>
+        <v>2075.0574273255816</v>
       </c>
       <c r="E22" s="1">
         <f>E21*E23</f>
-        <v>3626.1634659156975</v>
+        <v>3466.1556218023252</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="9"/>
-        <v>5734.0373237354661</v>
+        <f t="shared" si="8"/>
+        <v>5510.1554370348831</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="9"/>
-        <v>7734.8070599389539</v>
+        <f t="shared" si="8"/>
+        <v>7448.2431895465106</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="9"/>
-        <v>13054.668613067442</v>
+        <f t="shared" si="8"/>
+        <v>12581.841935358141</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="9"/>
-        <v>10680.116864673255</v>
+        <f t="shared" si="8"/>
+        <v>10151.412828144186</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="9"/>
-        <v>14354.377036987793</v>
+        <f t="shared" si="8"/>
+        <v>13773.376762909304</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="9"/>
-        <v>17107.776018493896</v>
+        <f t="shared" si="8"/>
+        <v>16468.150881454651</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" si="9"/>
-        <v>20049.742951107415</v>
+        <f t="shared" si="8"/>
+        <v>19323.97108026221</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" si="9"/>
-        <v>15133.074963925799</v>
+        <f t="shared" si="8"/>
+        <v>14339.872168038082</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="9"/>
-        <v>21853.761609869878</v>
+        <f t="shared" si="8"/>
+        <v>20953.770677042296</v>
       </c>
       <c r="O22" s="1">
-        <f t="shared" si="9"/>
-        <v>26265.748828190754</v>
+        <f t="shared" si="8"/>
+        <v>25279.887082707191</v>
       </c>
       <c r="P22" s="1">
-        <f t="shared" si="9"/>
-        <v>30037.009879211651</v>
+        <f t="shared" si="8"/>
+        <v>28951.378425074523</v>
       </c>
       <c r="Q22" s="1">
-        <f t="shared" si="9"/>
-        <v>23274.4188930942</v>
+        <f t="shared" si="8"/>
+        <v>22057.710724165168</v>
       </c>
       <c r="R22" s="1">
-        <f t="shared" si="9"/>
-        <v>32521.378341895936</v>
+        <f t="shared" si="8"/>
+        <v>31182.297513245372</v>
       </c>
       <c r="S22" s="1">
-        <f t="shared" si="9"/>
-        <v>38999.958356994488</v>
+        <f t="shared" si="8"/>
+        <v>37534.737710111061</v>
       </c>
       <c r="T22" s="1">
-        <f t="shared" si="9"/>
-        <v>45449.783248264685</v>
+        <f t="shared" si="8"/>
+        <v>43807.82408761367</v>
       </c>
       <c r="U22" s="1">
-        <f t="shared" si="9"/>
-        <v>34373.620984597452</v>
+        <f t="shared" si="8"/>
+        <v>32578.339078690551</v>
       </c>
       <c r="V22" s="1">
-        <f t="shared" si="9"/>
-        <v>47027.315143461514</v>
+        <f t="shared" si="8"/>
+        <v>45090.418376554575</v>
       </c>
       <c r="W22" s="1">
-        <f t="shared" si="9"/>
-        <v>54383.243618242384</v>
+        <f t="shared" si="8"/>
+        <v>52343.062676649381</v>
       </c>
       <c r="X22" s="1">
-        <f t="shared" si="9"/>
-        <v>59000.039250981659</v>
+        <f t="shared" si="8"/>
+        <v>56875.739477859577</v>
       </c>
       <c r="Y22" s="1">
-        <f t="shared" si="9"/>
-        <v>41450.099858048969</v>
+        <f t="shared" si="8"/>
+        <v>39218.787180790256</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -2649,99 +2824,99 @@
       </c>
       <c r="B24" s="1">
         <f>B21*10%</f>
-        <v>110.67267441860466</v>
+        <v>106.61308139534884</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" ref="C24:Y24" si="10">C21*10%</f>
-        <v>396.57014534883723</v>
+        <f t="shared" ref="C24:Y24" si="9">C21*10%</f>
+        <v>381.54965116279072</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="10"/>
-        <v>862.11405377906976</v>
+        <f t="shared" si="9"/>
+        <v>830.02297093023265</v>
       </c>
       <c r="E24" s="1">
         <f>E21*10%</f>
-        <v>1208.7211553052327</v>
+        <v>1155.3852072674417</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="10"/>
-        <v>1911.3457745784888</v>
+        <f t="shared" si="9"/>
+        <v>1836.7184790116278</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="10"/>
-        <v>2578.2690199796516</v>
+        <f t="shared" si="9"/>
+        <v>2482.7477298488375</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="10"/>
-        <v>3263.6671532668606</v>
+        <f t="shared" si="9"/>
+        <v>3145.4604838395353</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="10"/>
-        <v>2670.0292161683137</v>
+        <f t="shared" si="9"/>
+        <v>2537.8532070360466</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="10"/>
-        <v>3588.5942592469482</v>
+        <f t="shared" si="9"/>
+        <v>3443.3441907273259</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="10"/>
-        <v>4276.944004623474</v>
+        <f t="shared" si="9"/>
+        <v>4117.0377203636626</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" si="10"/>
-        <v>5012.4357377768538</v>
+        <f t="shared" si="9"/>
+        <v>4830.9927700655526</v>
       </c>
       <c r="M24" s="1">
-        <f t="shared" si="10"/>
-        <v>3783.2687409814498</v>
+        <f t="shared" si="9"/>
+        <v>3584.9680420095206</v>
       </c>
       <c r="N24" s="1">
-        <f t="shared" si="10"/>
-        <v>5463.4404024674695</v>
+        <f t="shared" si="9"/>
+        <v>5238.4426692605739</v>
       </c>
       <c r="O24" s="1">
-        <f t="shared" si="10"/>
-        <v>6566.4372070476884</v>
+        <f t="shared" si="9"/>
+        <v>6319.9717706767979</v>
       </c>
       <c r="P24" s="1">
-        <f t="shared" si="10"/>
-        <v>7509.2524698029129</v>
+        <f t="shared" si="9"/>
+        <v>7237.8446062686307</v>
       </c>
       <c r="Q24" s="1">
-        <f t="shared" si="10"/>
-        <v>5818.60472327355</v>
+        <f t="shared" si="9"/>
+        <v>5514.4276810412921</v>
       </c>
       <c r="R24" s="1">
-        <f t="shared" si="10"/>
-        <v>8130.3445854739839</v>
+        <f t="shared" si="9"/>
+        <v>7795.574378311343</v>
       </c>
       <c r="S24" s="1">
-        <f t="shared" si="10"/>
-        <v>9749.989589248622</v>
+        <f t="shared" si="9"/>
+        <v>9383.6844275277654</v>
       </c>
       <c r="T24" s="1">
-        <f t="shared" si="10"/>
-        <v>11362.445812066171</v>
+        <f t="shared" si="9"/>
+        <v>10951.956021903417</v>
       </c>
       <c r="U24" s="1">
-        <f t="shared" si="10"/>
-        <v>8593.4052461493629</v>
+        <f t="shared" si="9"/>
+        <v>8144.5847696726378</v>
       </c>
       <c r="V24" s="1">
-        <f t="shared" si="10"/>
-        <v>11756.828785865378</v>
+        <f t="shared" si="9"/>
+        <v>11272.604594138644</v>
       </c>
       <c r="W24" s="1">
-        <f t="shared" si="10"/>
-        <v>13595.810904560596</v>
+        <f t="shared" si="9"/>
+        <v>13085.765669162345</v>
       </c>
       <c r="X24" s="1">
-        <f t="shared" si="10"/>
-        <v>14750.009812745415</v>
+        <f t="shared" si="9"/>
+        <v>14218.934869464894</v>
       </c>
       <c r="Y24" s="1">
-        <f t="shared" si="10"/>
-        <v>10362.524964512242</v>
+        <f t="shared" si="9"/>
+        <v>9804.6967951975639</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -2750,99 +2925,99 @@
       </c>
       <c r="B25" s="9">
         <f>B21-B22-B24</f>
-        <v>774.70872093023263</v>
+        <v>746.29156976744184</v>
       </c>
       <c r="C25" s="9">
-        <f t="shared" ref="C25:Y25" si="11">C21-C22-C24</f>
-        <v>2577.7059447674419</v>
+        <f t="shared" ref="C25:Y25" si="10">C21-C22-C24</f>
+        <v>2480.0727325581397</v>
       </c>
       <c r="D25" s="9">
-        <f t="shared" si="11"/>
-        <v>5603.741349563953</v>
+        <f t="shared" si="10"/>
+        <v>5395.1493110465117</v>
       </c>
       <c r="E25" s="9">
         <f>E21-E22-E24</f>
-        <v>7252.326931831396</v>
+        <v>6932.3112436046504</v>
       </c>
       <c r="F25" s="9">
-        <f t="shared" si="11"/>
-        <v>11468.074647470932</v>
+        <f t="shared" si="10"/>
+        <v>11020.310874069766</v>
       </c>
       <c r="G25" s="9">
-        <f t="shared" si="11"/>
-        <v>15469.614119877908</v>
+        <f t="shared" si="10"/>
+        <v>14896.486379093025</v>
       </c>
       <c r="H25" s="9">
-        <f t="shared" si="11"/>
-        <v>16318.335766334303</v>
+        <f t="shared" si="10"/>
+        <v>15727.302419197673</v>
       </c>
       <c r="I25" s="9">
-        <f t="shared" si="11"/>
-        <v>13350.146080841569</v>
+        <f t="shared" si="10"/>
+        <v>12689.26603518023</v>
       </c>
       <c r="J25" s="9">
-        <f t="shared" si="11"/>
-        <v>17942.97129623474</v>
+        <f t="shared" si="10"/>
+        <v>17216.720953636624</v>
       </c>
       <c r="K25" s="9">
-        <f t="shared" si="11"/>
-        <v>21384.72002311737</v>
+        <f t="shared" si="10"/>
+        <v>20585.188601818314</v>
       </c>
       <c r="L25" s="9">
-        <f t="shared" si="11"/>
-        <v>25062.178688884269</v>
+        <f t="shared" si="10"/>
+        <v>24154.963850327757</v>
       </c>
       <c r="M25" s="9">
-        <f t="shared" si="11"/>
-        <v>18916.343704907249</v>
+        <f t="shared" si="10"/>
+        <v>17924.840210047598</v>
       </c>
       <c r="N25" s="9">
-        <f t="shared" si="11"/>
-        <v>27317.20201233734</v>
+        <f t="shared" si="10"/>
+        <v>26192.213346302862</v>
       </c>
       <c r="O25" s="9">
-        <f t="shared" si="11"/>
-        <v>32832.186035238432</v>
+        <f t="shared" si="10"/>
+        <v>31599.858853383979</v>
       </c>
       <c r="P25" s="9">
-        <f t="shared" si="11"/>
-        <v>37546.262349014563</v>
+        <f t="shared" si="10"/>
+        <v>36189.22303134315</v>
       </c>
       <c r="Q25" s="9">
-        <f t="shared" si="11"/>
-        <v>29093.02361636774</v>
+        <f t="shared" si="10"/>
+        <v>27572.13840520646</v>
       </c>
       <c r="R25" s="9">
-        <f t="shared" si="11"/>
-        <v>40651.722927369919</v>
+        <f t="shared" si="10"/>
+        <v>38977.871891556715</v>
       </c>
       <c r="S25" s="9">
-        <f t="shared" si="11"/>
-        <v>48749.947946243097</v>
+        <f t="shared" si="10"/>
+        <v>46918.422137638816</v>
       </c>
       <c r="T25" s="9">
-        <f t="shared" si="11"/>
-        <v>56812.229060330836</v>
+        <f t="shared" si="10"/>
+        <v>54759.780109517073</v>
       </c>
       <c r="U25" s="9">
-        <f t="shared" si="11"/>
-        <v>42967.026230746815</v>
+        <f t="shared" si="10"/>
+        <v>40722.923848363178</v>
       </c>
       <c r="V25" s="9">
-        <f t="shared" si="11"/>
-        <v>58784.143929326892</v>
+        <f t="shared" si="10"/>
+        <v>56363.022970693215</v>
       </c>
       <c r="W25" s="9">
-        <f t="shared" si="11"/>
-        <v>67979.054522802981</v>
+        <f t="shared" si="10"/>
+        <v>65428.828345811722</v>
       </c>
       <c r="X25" s="9">
-        <f t="shared" si="11"/>
-        <v>73750.04906372707</v>
+        <f t="shared" si="10"/>
+        <v>71094.674347324471</v>
       </c>
       <c r="Y25" s="9">
-        <f t="shared" si="11"/>
-        <v>51812.624822561207</v>
+        <f t="shared" si="10"/>
+        <v>49023.483975987809</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
@@ -2858,91 +3033,91 @@
         <v>44175</v>
       </c>
       <c r="D27" s="16">
-        <f t="shared" ref="D27:Y27" si="12">D11*12</f>
+        <f t="shared" ref="D27:Y27" si="11">D11*12</f>
         <v>82650</v>
       </c>
       <c r="E27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>121837.5</v>
       </c>
       <c r="F27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>161025</v>
       </c>
       <c r="G27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>193087.5</v>
       </c>
       <c r="H27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>231562.5</v>
       </c>
       <c r="I27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>277875</v>
       </c>
       <c r="J27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>303525</v>
       </c>
       <c r="K27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>334162.5</v>
       </c>
       <c r="L27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>386887.5</v>
       </c>
       <c r="M27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>413250</v>
       </c>
       <c r="N27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>479512.5</v>
       </c>
       <c r="O27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>514425</v>
       </c>
       <c r="P27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>567150</v>
       </c>
       <c r="Q27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>643387.5</v>
       </c>
       <c r="R27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>700387.5</v>
       </c>
       <c r="S27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>762375</v>
       </c>
       <c r="T27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>867825</v>
       </c>
       <c r="U27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>934800</v>
       </c>
       <c r="V27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>997500</v>
       </c>
       <c r="W27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1031700</v>
       </c>
       <c r="X27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1063050</v>
       </c>
       <c r="Y27" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1122900</v>
       </c>
     </row>
@@ -2951,95 +3126,95 @@
         <v>86</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" ref="C28:Y28" si="13">C27/B27</f>
+        <f t="shared" ref="C28:Y28" si="12">C27/B27</f>
         <v>3.1</v>
       </c>
       <c r="D28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.8709677419354838</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.4741379310344827</v>
       </c>
       <c r="F28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.3216374269005848</v>
       </c>
       <c r="G28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.1991150442477876</v>
       </c>
       <c r="H28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.1992619926199262</v>
       </c>
       <c r="I28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.2</v>
       </c>
       <c r="J28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.0923076923076922</v>
       </c>
       <c r="K28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.1009389671361502</v>
       </c>
       <c r="L28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.1577825159914712</v>
       </c>
       <c r="M28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.0681399631675874</v>
       </c>
       <c r="N28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.1603448275862069</v>
       </c>
       <c r="O28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.0728083209509658</v>
       </c>
       <c r="P28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.1024930747922437</v>
       </c>
       <c r="Q28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.1344221105527639</v>
       </c>
       <c r="R28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.0885935769656701</v>
       </c>
       <c r="S28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.0885045778229909</v>
       </c>
       <c r="T28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.1383177570093459</v>
       </c>
       <c r="U28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.0771756978653531</v>
       </c>
       <c r="V28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.0670731707317074</v>
       </c>
       <c r="W28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.0342857142857143</v>
       </c>
       <c r="X28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.0303867403314917</v>
       </c>
       <c r="Y28" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.0563002680965148</v>
       </c>
     </row>
@@ -3079,99 +3254,99 @@
         <v>44</v>
       </c>
       <c r="B33" s="15">
-        <f t="shared" ref="B33:Y33" si="14">B8</f>
+        <f t="shared" ref="B33:Y33" si="13">B8</f>
         <v>50</v>
       </c>
       <c r="C33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>200</v>
       </c>
       <c r="D33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>350</v>
       </c>
       <c r="E33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>500</v>
       </c>
       <c r="F33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>650</v>
       </c>
       <c r="G33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>700</v>
       </c>
       <c r="H33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>850</v>
       </c>
       <c r="I33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1000</v>
       </c>
       <c r="J33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1100</v>
       </c>
       <c r="K33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1200</v>
       </c>
       <c r="L33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1400</v>
       </c>
       <c r="M33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1500</v>
       </c>
       <c r="N33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1650</v>
       </c>
       <c r="O33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1750</v>
       </c>
       <c r="P33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1950</v>
       </c>
       <c r="Q33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2200</v>
       </c>
       <c r="R33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2400</v>
       </c>
       <c r="S33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2600</v>
       </c>
       <c r="T33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2800</v>
       </c>
       <c r="U33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>3000</v>
       </c>
       <c r="V33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>3200</v>
       </c>
       <c r="W33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>3300</v>
       </c>
       <c r="X33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>3400</v>
       </c>
       <c r="Y33" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>3600</v>
       </c>
     </row>
@@ -3257,99 +3432,99 @@
         <v>54</v>
       </c>
       <c r="B35">
-        <f t="shared" ref="B35:F35" si="15">ROUND(B33/B34,0)</f>
+        <f t="shared" ref="B35:G35" si="14">ROUND(B33/B34,0)</f>
         <v>50</v>
       </c>
       <c r="C35">
+        <f t="shared" si="14"/>
+        <v>200</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="14"/>
+        <v>350</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="14"/>
+        <v>500</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="14"/>
+        <v>650</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="14"/>
+        <v>778</v>
+      </c>
+      <c r="H35">
+        <f t="shared" ref="H35:Y35" si="15">ROUND(H33/H34,0)</f>
+        <v>944</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="15"/>
-        <v>200</v>
-      </c>
-      <c r="D35">
+        <v>1111</v>
+      </c>
+      <c r="J35">
         <f t="shared" si="15"/>
-        <v>350</v>
-      </c>
-      <c r="E35">
+        <v>1222</v>
+      </c>
+      <c r="K35">
         <f t="shared" si="15"/>
-        <v>500</v>
-      </c>
-      <c r="F35">
+        <v>1333</v>
+      </c>
+      <c r="L35">
         <f t="shared" si="15"/>
-        <v>650</v>
-      </c>
-      <c r="G35">
-        <f>ROUND(G33/G34,0)</f>
-        <v>778</v>
-      </c>
-      <c r="H35">
-        <f t="shared" ref="H35:Y35" si="16">ROUND(H33/H34,0)</f>
-        <v>944</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="16"/>
-        <v>1111</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="16"/>
-        <v>1222</v>
-      </c>
-      <c r="K35">
-        <f t="shared" si="16"/>
-        <v>1333</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="16"/>
         <v>1556</v>
       </c>
       <c r="M35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>1667</v>
       </c>
       <c r="N35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>1941</v>
       </c>
       <c r="O35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2059</v>
       </c>
       <c r="P35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2294</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2588</v>
       </c>
       <c r="R35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2824</v>
       </c>
       <c r="S35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>3059</v>
       </c>
       <c r="T35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>3500</v>
       </c>
       <c r="U35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>3750</v>
       </c>
       <c r="V35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>4000</v>
       </c>
       <c r="W35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>4125</v>
       </c>
       <c r="X35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>4250</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>4500</v>
       </c>
     </row>
@@ -3540,95 +3715,95 @@
         <v>2</v>
       </c>
       <c r="C39">
-        <f t="shared" ref="C39:Y39" si="17">ROUND(C35*C38,0)</f>
+        <f t="shared" ref="C39:Y39" si="16">ROUND(C35*C38,0)</f>
         <v>6</v>
       </c>
       <c r="D39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="E39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>16</v>
       </c>
       <c r="F39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>21</v>
       </c>
       <c r="G39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>25</v>
       </c>
       <c r="H39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>30</v>
       </c>
       <c r="I39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>36</v>
       </c>
       <c r="J39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>39</v>
       </c>
       <c r="K39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>43</v>
       </c>
       <c r="L39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>50</v>
       </c>
       <c r="M39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>53</v>
       </c>
       <c r="N39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>62</v>
       </c>
       <c r="O39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>66</v>
       </c>
       <c r="P39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>73</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>83</v>
       </c>
       <c r="R39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>90</v>
       </c>
       <c r="S39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>98</v>
       </c>
       <c r="T39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>112</v>
       </c>
       <c r="U39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>120</v>
       </c>
       <c r="V39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>128</v>
       </c>
       <c r="W39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>132</v>
       </c>
       <c r="X39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>136</v>
       </c>
       <c r="Y39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>144</v>
       </c>
     </row>
@@ -3649,87 +3824,87 @@
         <v>6531.25</v>
       </c>
       <c r="E41" s="9">
-        <f t="shared" ref="E41:M41" si="18">E37*E39</f>
+        <f t="shared" ref="E41:M41" si="17">E37*E39</f>
         <v>9500</v>
       </c>
       <c r="F41" s="9">
+        <f t="shared" si="17"/>
+        <v>12468.75</v>
+      </c>
+      <c r="G41" s="9">
+        <f t="shared" si="17"/>
+        <v>14843.75</v>
+      </c>
+      <c r="H41" s="9">
+        <f t="shared" si="17"/>
+        <v>17812.5</v>
+      </c>
+      <c r="I41" s="9">
+        <f t="shared" si="17"/>
+        <v>21375</v>
+      </c>
+      <c r="J41" s="9">
+        <f t="shared" si="17"/>
+        <v>23156.25</v>
+      </c>
+      <c r="K41" s="9">
+        <f t="shared" si="17"/>
+        <v>25531.25</v>
+      </c>
+      <c r="L41" s="9">
+        <f t="shared" si="17"/>
+        <v>29687.5</v>
+      </c>
+      <c r="M41" s="9">
+        <f t="shared" si="17"/>
+        <v>31468.75</v>
+      </c>
+      <c r="N41" s="9">
+        <f t="shared" ref="N41:Y41" si="18">N37*N39</f>
+        <v>36812.5</v>
+      </c>
+      <c r="O41" s="9">
         <f t="shared" si="18"/>
-        <v>12468.75</v>
-      </c>
-      <c r="G41" s="9">
+        <v>39187.5</v>
+      </c>
+      <c r="P41" s="9">
         <f t="shared" si="18"/>
-        <v>14843.75</v>
-      </c>
-      <c r="H41" s="9">
+        <v>43343.75</v>
+      </c>
+      <c r="Q41" s="9">
         <f t="shared" si="18"/>
-        <v>17812.5</v>
-      </c>
-      <c r="I41" s="9">
+        <v>49281.25</v>
+      </c>
+      <c r="R41" s="9">
         <f t="shared" si="18"/>
-        <v>21375</v>
-      </c>
-      <c r="J41" s="9">
+        <v>53437.5</v>
+      </c>
+      <c r="S41" s="9">
         <f t="shared" si="18"/>
-        <v>23156.25</v>
-      </c>
-      <c r="K41" s="9">
+        <v>58187.5</v>
+      </c>
+      <c r="T41" s="9">
         <f t="shared" si="18"/>
-        <v>25531.25</v>
-      </c>
-      <c r="L41" s="9">
+        <v>66500</v>
+      </c>
+      <c r="U41" s="9">
         <f t="shared" si="18"/>
-        <v>29687.5</v>
-      </c>
-      <c r="M41" s="9">
+        <v>71250</v>
+      </c>
+      <c r="V41" s="9">
         <f t="shared" si="18"/>
-        <v>31468.75</v>
-      </c>
-      <c r="N41" s="9">
-        <f t="shared" ref="N41:Y41" si="19">N37*N39</f>
-        <v>36812.5</v>
-      </c>
-      <c r="O41" s="9">
-        <f t="shared" si="19"/>
-        <v>39187.5</v>
-      </c>
-      <c r="P41" s="9">
-        <f t="shared" si="19"/>
-        <v>43343.75</v>
-      </c>
-      <c r="Q41" s="9">
-        <f t="shared" si="19"/>
-        <v>49281.25</v>
-      </c>
-      <c r="R41" s="9">
-        <f t="shared" si="19"/>
-        <v>53437.5</v>
-      </c>
-      <c r="S41" s="9">
-        <f t="shared" si="19"/>
-        <v>58187.5</v>
-      </c>
-      <c r="T41" s="9">
-        <f t="shared" si="19"/>
-        <v>66500</v>
-      </c>
-      <c r="U41" s="9">
-        <f t="shared" si="19"/>
-        <v>71250</v>
-      </c>
-      <c r="V41" s="9">
-        <f t="shared" si="19"/>
         <v>76000</v>
       </c>
       <c r="W41" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>78375</v>
       </c>
       <c r="X41" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>80750</v>
       </c>
       <c r="Y41" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>85500</v>
       </c>
     </row>
@@ -3825,87 +4000,87 @@
         <v>356.25000000000006</v>
       </c>
       <c r="E47" s="9">
-        <f t="shared" ref="E47:M47" si="20">D39*E46*D37</f>
+        <f t="shared" ref="E47:M47" si="19">D39*E46*D37</f>
         <v>653.125</v>
       </c>
       <c r="F47" s="9">
+        <f t="shared" si="19"/>
+        <v>950</v>
+      </c>
+      <c r="G47" s="9">
+        <f t="shared" si="19"/>
+        <v>1246.875</v>
+      </c>
+      <c r="H47" s="9">
+        <f t="shared" si="19"/>
+        <v>1484.375</v>
+      </c>
+      <c r="I47" s="9">
+        <f t="shared" si="19"/>
+        <v>1781.25</v>
+      </c>
+      <c r="J47" s="9">
+        <f t="shared" si="19"/>
+        <v>2137.5</v>
+      </c>
+      <c r="K47" s="9">
+        <f t="shared" si="19"/>
+        <v>2315.625</v>
+      </c>
+      <c r="L47" s="9">
+        <f t="shared" si="19"/>
+        <v>2553.125</v>
+      </c>
+      <c r="M47" s="9">
+        <f t="shared" si="19"/>
+        <v>2968.75</v>
+      </c>
+      <c r="N47" s="9">
+        <f t="shared" ref="N47:Y47" si="20">M39*N46*M37</f>
+        <v>3146.8750000000005</v>
+      </c>
+      <c r="O47" s="9">
         <f t="shared" si="20"/>
-        <v>950</v>
-      </c>
-      <c r="G47" s="9">
+        <v>3681.25</v>
+      </c>
+      <c r="P47" s="9">
         <f t="shared" si="20"/>
-        <v>1246.875</v>
-      </c>
-      <c r="H47" s="9">
+        <v>3918.7500000000005</v>
+      </c>
+      <c r="Q47" s="9">
         <f t="shared" si="20"/>
-        <v>1484.375</v>
-      </c>
-      <c r="I47" s="9">
+        <v>4334.375</v>
+      </c>
+      <c r="R47" s="9">
         <f t="shared" si="20"/>
-        <v>1781.25</v>
-      </c>
-      <c r="J47" s="9">
+        <v>4928.125</v>
+      </c>
+      <c r="S47" s="9">
         <f t="shared" si="20"/>
-        <v>2137.5</v>
-      </c>
-      <c r="K47" s="9">
+        <v>5343.75</v>
+      </c>
+      <c r="T47" s="9">
         <f t="shared" si="20"/>
-        <v>2315.625</v>
-      </c>
-      <c r="L47" s="9">
+        <v>5818.75</v>
+      </c>
+      <c r="U47" s="9">
         <f t="shared" si="20"/>
-        <v>2553.125</v>
-      </c>
-      <c r="M47" s="9">
+        <v>6650.0000000000009</v>
+      </c>
+      <c r="V47" s="9">
         <f t="shared" si="20"/>
-        <v>2968.75</v>
-      </c>
-      <c r="N47" s="9">
-        <f t="shared" ref="N47" si="21">M39*N46*M37</f>
-        <v>3146.8750000000005</v>
-      </c>
-      <c r="O47" s="9">
-        <f t="shared" ref="O47" si="22">N39*O46*N37</f>
-        <v>3681.25</v>
-      </c>
-      <c r="P47" s="9">
-        <f t="shared" ref="P47" si="23">O39*P46*O37</f>
-        <v>3918.7500000000005</v>
-      </c>
-      <c r="Q47" s="9">
-        <f t="shared" ref="Q47" si="24">P39*Q46*P37</f>
-        <v>4334.375</v>
-      </c>
-      <c r="R47" s="9">
-        <f t="shared" ref="R47" si="25">Q39*R46*Q37</f>
-        <v>4928.125</v>
-      </c>
-      <c r="S47" s="9">
-        <f t="shared" ref="S47" si="26">R39*S46*R37</f>
-        <v>5343.75</v>
-      </c>
-      <c r="T47" s="9">
-        <f t="shared" ref="T47" si="27">S39*T46*S37</f>
-        <v>5818.75</v>
-      </c>
-      <c r="U47" s="9">
-        <f t="shared" ref="U47" si="28">T39*U46*T37</f>
-        <v>6650.0000000000009</v>
-      </c>
-      <c r="V47" s="9">
-        <f t="shared" ref="V47" si="29">U39*V46*U37</f>
         <v>7125</v>
       </c>
       <c r="W47" s="9">
-        <f t="shared" ref="W47" si="30">V39*W46*V37</f>
+        <f t="shared" si="20"/>
         <v>7600</v>
       </c>
       <c r="X47" s="9">
-        <f t="shared" ref="X47" si="31">W39*X46*W37</f>
+        <f t="shared" si="20"/>
         <v>7837.5000000000009</v>
       </c>
       <c r="Y47" s="9">
-        <f t="shared" ref="Y47" si="32">X39*Y46*X37</f>
+        <f t="shared" si="20"/>
         <v>8075.0000000000009</v>
       </c>
     </row>
@@ -3957,7 +4132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7B0D58-8F04-4886-8C8E-354108E90D0C}">
   <dimension ref="C5:J14"/>
   <sheetViews>

</xml_diff>